<commit_message>
solver_diff/ fix bugs regression2
</commit_message>
<xml_diff>
--- a/exemplos_tutorial_quimica_nova/exemplo4.xlsx
+++ b/exemplos_tutorial_quimica_nova/exemplo4.xlsx
@@ -8,24 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documentos\UFSCar\TCC\playlist23\exemplos_tutorial_quimica_nova\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13044349-ECFE-4525-9BDE-C8A77BB89C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4F95BA-95D8-4640-8B33-452545908090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>v1</t>
   </si>
@@ -52,6 +60,51 @@
   </si>
   <si>
     <t>Rend (%)</t>
+  </si>
+  <si>
+    <t>b0</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>b3</t>
+  </si>
+  <si>
+    <t>b4</t>
+  </si>
+  <si>
+    <t>b12</t>
+  </si>
+  <si>
+    <t>b11</t>
+  </si>
+  <si>
+    <t>b22</t>
+  </si>
+  <si>
+    <t>b33</t>
+  </si>
+  <si>
+    <t>b44</t>
+  </si>
+  <si>
+    <t>b13</t>
+  </si>
+  <si>
+    <t>b14</t>
+  </si>
+  <si>
+    <t>b23</t>
+  </si>
+  <si>
+    <t>b24</t>
+  </si>
+  <si>
+    <t>b34</t>
   </si>
 </sst>
 </file>
@@ -369,15 +422,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:X30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -405,8 +458,53 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-1</v>
       </c>
@@ -434,8 +532,67 @@
       <c r="I2">
         <v>73</v>
       </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <f>A2</f>
+        <v>-1</v>
+      </c>
+      <c r="L2">
+        <f>C2</f>
+        <v>-1</v>
+      </c>
+      <c r="M2">
+        <f>E2</f>
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <f>G2</f>
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f>K2^2</f>
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <f>L2^2</f>
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <f>M2^2</f>
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <f>N2^2</f>
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <f>K2*L2</f>
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <f>K2*M2</f>
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <f>K2*N2</f>
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <f>L2*M2</f>
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <f>L2*N2</f>
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <f>M2*N2</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -463,8 +620,67 @@
       <c r="I3">
         <v>88.15</v>
       </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K30" si="0">A3</f>
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L30" si="1">C3</f>
+        <v>-1</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M30" si="2">E3</f>
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N30" si="3">G3</f>
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O30" si="4">K3^2</f>
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P30" si="5">L3^2</f>
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q30" si="6">M3^2</f>
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R30" si="7">N3^2</f>
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ref="S3:S30" si="8">K3*L3</f>
+        <v>-1</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T30" si="9">K3*M3</f>
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <f t="shared" ref="U3:U30" si="10">K3*N3</f>
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <f t="shared" ref="V3:V30" si="11">L3*M3</f>
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <f t="shared" ref="W3:W30" si="12">L3*N3</f>
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <f t="shared" ref="X3:X30" si="13">M3*N3</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-1</v>
       </c>
@@ -492,8 +708,67 @@
       <c r="I4">
         <v>80.98</v>
       </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="8"/>
+        <v>-1</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -521,8 +796,67 @@
       <c r="I5">
         <v>90.82</v>
       </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -550,8 +884,67 @@
       <c r="I6">
         <v>84.55</v>
       </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -579,8 +972,67 @@
       <c r="I7">
         <v>88.23</v>
       </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="13"/>
+        <v>-1</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -608,8 +1060,67 @@
       <c r="I8">
         <v>86.86</v>
       </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="13"/>
+        <v>-1</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -637,8 +1148,67 @@
       <c r="I9">
         <v>91.41</v>
       </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-1</v>
       </c>
@@ -666,8 +1236,67 @@
       <c r="I10">
         <v>75.38</v>
       </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -695,8 +1324,67 @@
       <c r="I11">
         <v>88.5</v>
       </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="10"/>
+        <v>-1</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>-1</v>
       </c>
@@ -724,8 +1412,67 @@
       <c r="I12">
         <v>80.239999999999995</v>
       </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="10"/>
+        <v>-1</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -753,8 +1500,67 @@
       <c r="I13">
         <v>94.13</v>
       </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -782,8 +1588,67 @@
       <c r="I14">
         <v>80.17</v>
       </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -811,8 +1676,67 @@
       <c r="I15">
         <v>88.09</v>
       </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="11"/>
+        <v>-1</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -840,8 +1764,67 @@
       <c r="I16">
         <v>91.47</v>
       </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="11"/>
+        <v>-1</v>
+      </c>
+      <c r="W16">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -869,8 +1852,67 @@
       <c r="I17">
         <v>90.03</v>
       </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="W17">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>-1</v>
       </c>
@@ -898,8 +1940,67 @@
       <c r="I18">
         <v>72.34</v>
       </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="U18">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -927,8 +2028,67 @@
       <c r="I19">
         <v>89.63</v>
       </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="9"/>
+        <v>-1</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>-1</v>
       </c>
@@ -956,8 +2116,67 @@
       <c r="I20">
         <v>84.61</v>
       </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="9"/>
+        <v>-1</v>
+      </c>
+      <c r="U20">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X20">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -985,8 +2204,67 @@
       <c r="I21">
         <v>89.31</v>
       </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="R21">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="U21">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -1014,8 +2292,67 @@
       <c r="I22">
         <v>79.08</v>
       </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="X22">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -1043,8 +2380,67 @@
       <c r="I23">
         <v>88.3</v>
       </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <f t="shared" si="12"/>
+        <v>-1</v>
+      </c>
+      <c r="X23">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
@@ -1072,8 +2468,67 @@
       <c r="I24">
         <v>88.02</v>
       </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <f t="shared" si="12"/>
+        <v>-1</v>
+      </c>
+      <c r="X24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -1101,8 +2556,67 @@
       <c r="I25">
         <v>87.29</v>
       </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="X25">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -1130,8 +2644,67 @@
       <c r="I26">
         <v>91.61</v>
       </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="W26">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X26">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0</v>
       </c>
@@ -1159,8 +2732,67 @@
       <c r="I27">
         <v>91.7</v>
       </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0</v>
       </c>
@@ -1188,8 +2820,67 @@
       <c r="I28">
         <v>93</v>
       </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X28">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0</v>
       </c>
@@ -1217,8 +2908,67 @@
       <c r="I29">
         <v>92.11</v>
       </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V29">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="W29">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X29">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0</v>
       </c>
@@ -1245,6 +2995,65 @@
       </c>
       <c r="I30">
         <v>93</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X30">
+        <f t="shared" si="13"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>